<commit_message>
Commit on Fri Jul  8 00:20:01 IST 2022
</commit_message>
<xml_diff>
--- a/paper_material/result/feature_scores.xlsx
+++ b/paper_material/result/feature_scores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13335" windowHeight="12315"/>
+    <workbookView windowWidth="27795" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>score</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Dropping Optical/UV features</t>
   </si>
   <si>
-    <t>Dropping MW features</t>
-  </si>
-  <si>
     <t>Dropping Color features</t>
   </si>
 </sst>
@@ -83,7 +80,7 @@
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +90,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -549,152 +555,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -712,6 +718,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1038,10 +1050,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -1063,7 +1075,7 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1074,16 +1086,16 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5"/>
@@ -1146,7 +1158,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1161,7 +1173,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1176,7 +1188,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1203,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="6"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1206,16 +1218,16 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1230,7 +1242,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="6"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1245,7 +1257,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="6"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1272,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="6"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1287,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="6"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1290,7 +1302,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="6"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1305,7 +1317,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="6"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1320,7 +1332,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="6"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1335,16 +1347,16 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="6"/>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="6"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1359,7 +1371,7 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="6"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1374,7 +1386,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="6"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1389,7 +1401,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="6"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1404,7 +1416,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="6"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +1431,7 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="6"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -1434,7 +1446,7 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="6"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
@@ -1449,7 +1461,7 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="6"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1464,16 +1476,16 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="6"/>
-      <c r="B30" s="1" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="6"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1488,7 +1500,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="6"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1503,7 +1515,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="6"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
@@ -1518,7 +1530,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="6"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1533,7 +1545,7 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="6"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1" t="s">
         <v>10</v>
       </c>
@@ -1548,7 +1560,7 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="6"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
@@ -1563,7 +1575,7 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="6"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
@@ -1578,7 +1590,7 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="6"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
@@ -1592,58 +1604,55 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="6"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C40">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="D40">
-        <v>0.91</v>
+        <v>0.97</v>
       </c>
       <c r="E40">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="6"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C41">
-        <v>0.88</v>
+        <v>0.95</v>
       </c>
       <c r="D41">
-        <v>0.89</v>
+        <v>0.96</v>
       </c>
       <c r="E41">
-        <v>0.89</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="6"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C42">
-        <v>0.9</v>
+        <v>0.96</v>
       </c>
       <c r="D42">
-        <v>0.83</v>
+        <v>0.92</v>
       </c>
       <c r="E42">
-        <v>0.86</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="43" spans="2:5">
@@ -1651,7 +1660,7 @@
         <v>9</v>
       </c>
       <c r="C43">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="D43">
         <v>0.91</v>
@@ -1665,13 +1674,13 @@
         <v>10</v>
       </c>
       <c r="C44">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="D44">
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="E44">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="45" spans="2:5">
@@ -1679,13 +1688,13 @@
         <v>11</v>
       </c>
       <c r="C45">
-        <v>0.43</v>
+        <v>0.72</v>
       </c>
       <c r="D45">
-        <v>0.61</v>
+        <v>0.73</v>
       </c>
       <c r="E45">
-        <v>0.5</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="46" spans="2:5">
@@ -1693,13 +1702,13 @@
         <v>12</v>
       </c>
       <c r="C46">
-        <v>0.48</v>
+        <v>0.55</v>
       </c>
       <c r="D46">
-        <v>0.56</v>
+        <v>0.59</v>
       </c>
       <c r="E46">
-        <v>0.52</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="47" spans="2:5">
@@ -1707,139 +1716,21 @@
         <v>13</v>
       </c>
       <c r="C47">
-        <v>0.21</v>
+        <v>0.41</v>
       </c>
       <c r="D47">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="E47">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49">
-        <v>0.97</v>
-      </c>
-      <c r="D49">
-        <v>0.97</v>
-      </c>
-      <c r="E49">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50">
-        <v>0.95</v>
-      </c>
-      <c r="D50">
-        <v>0.96</v>
-      </c>
-      <c r="E50">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51">
-        <v>0.96</v>
-      </c>
-      <c r="D51">
-        <v>0.92</v>
-      </c>
-      <c r="E51">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52">
-        <v>0.91</v>
-      </c>
-      <c r="D52">
-        <v>0.91</v>
-      </c>
-      <c r="E52">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53">
-        <v>0.8</v>
-      </c>
-      <c r="D53">
-        <v>0.94</v>
-      </c>
-      <c r="E53">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5">
-      <c r="B54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54">
-        <v>0.72</v>
-      </c>
-      <c r="D54">
-        <v>0.73</v>
-      </c>
-      <c r="E54">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="B55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55">
-        <v>0.55</v>
-      </c>
-      <c r="D55">
-        <v>0.59</v>
-      </c>
-      <c r="E55">
-        <v>0.57</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5">
-      <c r="B56" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56">
-        <v>0.41</v>
-      </c>
-      <c r="D56">
-        <v>0.38</v>
-      </c>
-      <c r="E56">
         <v>0.39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B39:E39"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>

</xml_diff>

<commit_message>
Commit on Fri Jul  8 00:30:01 IST 2022
</commit_message>
<xml_diff>
--- a/paper_material/result/feature_scores.xlsx
+++ b/paper_material/result/feature_scores.xlsx
@@ -1052,8 +1052,8 @@
   <sheetPr/>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75" outlineLevelCol="4"/>

</xml_diff>